<commit_message>
Added CommProtocol.c and CommProtocol.h
</commit_message>
<xml_diff>
--- a/Communications Protocol/Command Structure.xlsx
+++ b/Communications Protocol/Command Structure.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Command</t>
   </si>
@@ -207,7 +207,31 @@
     <t>Sample Rate is built into the modes</t>
   </si>
   <si>
-    <t>Readdress</t>
+    <t>Readdress 1</t>
+  </si>
+  <si>
+    <t>Readdress 2</t>
+  </si>
+  <si>
+    <t>Readdress 3</t>
+  </si>
+  <si>
+    <t>Readdress 4</t>
+  </si>
+  <si>
+    <t>Readdress 5</t>
+  </si>
+  <si>
+    <t>Readdress 6</t>
+  </si>
+  <si>
+    <t>Readdress 7</t>
+  </si>
+  <si>
+    <t>Readdress 8</t>
+  </si>
+  <si>
+    <t>Is there another board?</t>
   </si>
 </sst>
 </file>
@@ -628,12 +652,12 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -840,41 +864,65 @@
       </c>
     </row>
     <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
       <c r="C24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
       <c r="C25" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
       <c r="C26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
       <c r="C27" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
       <c r="C28" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
       <c r="C29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
       <c r="C30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
       <c r="C31" t="s">
         <v>44</v>
       </c>

</xml_diff>